<commit_message>
Big update with local data
</commit_message>
<xml_diff>
--- a/Open Courses/Data_Structures/Data-Structures-Course-Schedule-Fabruary-2016.xlsx
+++ b/Open Courses/Data_Structures/Data-Structures-Course-Schedule-Fabruary-2016.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" tabRatio="264"/>
   </bookViews>
   <sheets>
     <sheet name="Data Structures - Schedule" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd"/>
   </numFmts>
@@ -467,6 +467,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -502,6 +519,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -681,22 +715,22 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>17</v>
       </c>
@@ -719,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -744,7 +778,7 @@
         <v>42423</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -769,7 +803,7 @@
         <v>42423</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -794,7 +828,7 @@
         <v>42425</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -819,7 +853,7 @@
         <v>42430</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -844,7 +878,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -869,7 +903,7 @@
         <v>42437</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -877,11 +911,11 @@
         <v>14</v>
       </c>
       <c r="C8" s="15">
-        <v>42432</v>
+        <v>42437</v>
       </c>
       <c r="D8" s="16">
         <f>Table13[[#This Row],[Date]]</f>
-        <v>42432</v>
+        <v>42437</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>4</v>
@@ -891,10 +925,10 @@
       </c>
       <c r="G8" s="15">
         <f>Table13[[#This Row],[Date]]+7</f>
-        <v>42439</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -902,11 +936,11 @@
         <v>19</v>
       </c>
       <c r="C9" s="15">
-        <v>42437</v>
+        <v>42438</v>
       </c>
       <c r="D9" s="16">
         <f>Table13[[#This Row],[Date]]</f>
-        <v>42437</v>
+        <v>42438</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>4</v>
@@ -916,10 +950,10 @@
       </c>
       <c r="G9" s="15">
         <f>Table13[[#This Row],[Date]]+7</f>
-        <v>42444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -944,7 +978,7 @@
         <v>42446</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -969,7 +1003,7 @@
         <v>42451</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -994,7 +1028,7 @@
         <v>42453</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1019,7 +1053,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>12</v>
       </c>

</xml_diff>